<commit_message>
add new parameter and change dateformate report name.
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -9,14 +9,15 @@
   <sheets>
     <sheet name="logininfo" sheetId="1" r:id="rId1"/>
     <sheet name="logininfo2" sheetId="4" r:id="rId2"/>
-    <sheet name="userinfo" sheetId="2" r:id="rId3"/>
+    <sheet name="userinfo2" sheetId="5" r:id="rId3"/>
+    <sheet name="userinfo" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="15">
   <si>
     <t>Admin</t>
   </si>
@@ -421,7 +422,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,9 +484,121 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>